<commit_message>
Update Controller Names and JPA Configuration
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minlwin/Desktop/clinic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minlwin/git/intern-web/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Schedule!$A$1:$I$35</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Controller Methods</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Android</t>
+  </si>
+  <si>
+    <t>PublicDoctorController.java</t>
+  </si>
+  <si>
+    <t>PublicHomeController.java</t>
+  </si>
+  <si>
+    <t>MemberBookingController.java</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -214,13 +223,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -967,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -983,31 +992,31 @@
         <v>43626</v>
       </c>
       <c r="C1" s="7">
-        <f>B1+7</f>
+        <f t="shared" ref="C1:I1" si="0">B1+7</f>
         <v>43633</v>
       </c>
       <c r="D1" s="7">
-        <f>C1+7</f>
+        <f t="shared" si="0"/>
         <v>43640</v>
       </c>
       <c r="E1" s="7">
-        <f>D1+7</f>
+        <f t="shared" si="0"/>
         <v>43647</v>
       </c>
       <c r="F1" s="7">
-        <f>E1+7</f>
+        <f t="shared" si="0"/>
         <v>43654</v>
       </c>
       <c r="G1" s="7">
-        <f>F1+7</f>
+        <f t="shared" si="0"/>
         <v>43661</v>
       </c>
       <c r="H1" s="7">
-        <f>G1+7</f>
+        <f t="shared" si="0"/>
         <v>43668</v>
       </c>
       <c r="I1" s="7">
-        <f>H1+7</f>
+        <f t="shared" si="0"/>
         <v>43675</v>
       </c>
       <c r="J1" s="2"/>
@@ -1184,11 +1193,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1280,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>26</v>
@@ -1298,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>32</v>
@@ -1406,7 +1415,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update Controller Methods and Schedules
</commit_message>
<xml_diff>
--- a/documents/schedule.xlsx
+++ b/documents/schedule.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3084E95D-49B7-4FD8-8983-4C5AE0822C65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI GAMING\git\intern-web\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFBC94D-FEA0-42A9-8E94-19140B38A535}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23064" windowHeight="13224" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -13,10 +18,9 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Schedule!$A$1:$I$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Schedule!$A$1:$I$47</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
-  <oleSize ref="A1:I21"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="58">
   <si>
     <t>Controller Methods</t>
   </si>
@@ -184,19 +188,28 @@
     <t>bookings.html</t>
   </si>
   <si>
-    <t>create-family.html</t>
-  </si>
-  <si>
     <t>family.html</t>
   </si>
   <si>
-    <t>familyMemberCreate.html</t>
-  </si>
-  <si>
-    <t>familyMemberUpdate.html</t>
-  </si>
-  <si>
     <t>home.html</t>
+  </si>
+  <si>
+    <t>family-edit.html</t>
+  </si>
+  <si>
+    <t>clinic-edit.html</t>
+  </si>
+  <si>
+    <t>clinic.html</t>
+  </si>
+  <si>
+    <t>doctor-edit.html</t>
+  </si>
+  <si>
+    <t>patient.html</t>
+  </si>
+  <si>
+    <t>patients.html</t>
   </si>
 </sst>
 </file>
@@ -1287,10 +1300,10 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1958,9 +1971,16 @@
       <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="5">
+        <v>43628</v>
+      </c>
+      <c r="G24" s="5">
+        <f>F24+2</f>
+        <v>43630</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
@@ -1978,9 +1998,16 @@
       <c r="D25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="E25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="5">
+        <v>43628</v>
+      </c>
+      <c r="G25" s="5">
+        <f>F25+2</f>
+        <v>43630</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
@@ -1998,9 +2025,16 @@
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="5">
+        <v>43630</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26+2</f>
+        <v>43632</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
@@ -2018,9 +2052,16 @@
       <c r="D27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="E27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="5">
+        <v>43627</v>
+      </c>
+      <c r="G27" s="5">
+        <f>F27+1</f>
+        <v>43628</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
@@ -2038,9 +2079,16 @@
       <c r="D28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="5">
+        <v>43627</v>
+      </c>
+      <c r="G28" s="5">
+        <f>F28+1</f>
+        <v>43628</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
@@ -2058,9 +2106,16 @@
       <c r="D29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="5">
+        <v>43628</v>
+      </c>
+      <c r="G29" s="5">
+        <f>F29+2</f>
+        <v>43630</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
@@ -2078,9 +2133,16 @@
       <c r="D30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="E30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="5">
+        <v>43627</v>
+      </c>
+      <c r="G30" s="5">
+        <f>F30+1</f>
+        <v>43628</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
@@ -2098,9 +2160,16 @@
       <c r="D31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="E31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="5">
+        <v>43628</v>
+      </c>
+      <c r="G31" s="5">
+        <f>F31+2</f>
+        <v>43630</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
@@ -2118,9 +2187,16 @@
       <c r="D32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="E32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="5">
+        <v>43630</v>
+      </c>
+      <c r="G32" s="5">
+        <f>F32+2</f>
+        <v>43632</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
@@ -2136,11 +2212,18 @@
         <v>20</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="5">
+        <v>43628</v>
+      </c>
+      <c r="G33" s="5">
+        <f>F33+2</f>
+        <v>43630</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
@@ -2156,11 +2239,18 @@
         <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="5">
+        <v>43630</v>
+      </c>
+      <c r="G34" s="5">
+        <f>F34+2</f>
+        <v>43632</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
@@ -2176,11 +2266,18 @@
         <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="5">
+        <v>43629</v>
+      </c>
+      <c r="G35" s="5">
+        <f>F35+2</f>
+        <v>43631</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
@@ -2193,14 +2290,21 @@
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="5">
+        <v>43628</v>
+      </c>
+      <c r="G36" s="5">
+        <f>F36+2</f>
+        <v>43630</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
@@ -2213,14 +2317,21 @@
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="5">
+        <v>43631</v>
+      </c>
+      <c r="G37" s="5">
+        <f>F37+2</f>
+        <v>43633</v>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
@@ -2229,14 +2340,25 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="D38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="5">
+        <v>43633</v>
+      </c>
+      <c r="G38" s="5">
+        <f>F38+2</f>
+        <v>43635</v>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
@@ -2245,12 +2367,25 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="B39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="5">
+        <v>43630</v>
+      </c>
+      <c r="G39" s="5">
+        <f>F39+2</f>
+        <v>43632</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
@@ -2259,12 +2394,25 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="B40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="5">
+        <v>43632</v>
+      </c>
+      <c r="G40" s="5">
+        <f>F40+2</f>
+        <v>43634</v>
+      </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
@@ -2273,12 +2421,25 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="5">
+        <v>43630</v>
+      </c>
+      <c r="G41" s="5">
+        <f>F41+2</f>
+        <v>43632</v>
+      </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
@@ -2287,12 +2448,25 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="B42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="5">
+        <v>43630</v>
+      </c>
+      <c r="G42" s="5">
+        <f>F42+2</f>
+        <v>43632</v>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
@@ -2301,12 +2475,25 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="B43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="5">
+        <v>43632</v>
+      </c>
+      <c r="G43" s="5">
+        <f>F43+2</f>
+        <v>43634</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
@@ -2315,12 +2502,25 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="5">
+        <v>43632</v>
+      </c>
+      <c r="G44" s="5">
+        <f>F44+2</f>
+        <v>43634</v>
+      </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
@@ -2411,7 +2611,7 @@
       <c r="I51" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I35" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:I47" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H51" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Not Yet, On Schedule, Delay, Complete"</formula1>

</xml_diff>